<commit_message>
Student And Teacher Services and fn done correctly
</commit_message>
<xml_diff>
--- a/DB/StudentDB.xlsx
+++ b/DB/StudentDB.xlsx
@@ -3,24 +3,102 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SchoolSystem\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B927F9-1BBE-4756-BA77-460B9B1BE91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846A54B8-A428-4B4E-AC37-FCDA4ACFE84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="168" windowWidth="12036" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7080" yWindow="168" windowWidth="15648" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Students Details " sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>Estimation</t>
+  </si>
+  <si>
+    <t>Parent's Email</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Courses</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>isAbsent</t>
+  </si>
+  <si>
+    <t>Student1</t>
+  </si>
+  <si>
+    <t>parents_Student1@gmail.com</t>
+  </si>
+  <si>
+    <t>1 Giza Egypt</t>
+  </si>
+  <si>
+    <t>[English, Math]</t>
+  </si>
+  <si>
+    <t>student2</t>
+  </si>
+  <si>
+    <t>parents_Strudent2@gmail.com</t>
+  </si>
+  <si>
+    <t>2 Cairo</t>
+  </si>
+  <si>
+    <t>[Arabic]</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>student5</t>
+  </si>
+  <si>
+    <t>parentStudent5@gmail</t>
+  </si>
+  <si>
+    <t>55 street</t>
+  </si>
+  <si>
+    <t>[Ar, En, Math, German]</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -365,13 +443,144 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE6583AD-CB73-41AC-AB9B-6055EEC84344}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>14</v>
+      </c>
+      <c r="I2">
+        <v>1111111111</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3">
+        <v>12</v>
+      </c>
+      <c r="I3">
+        <v>222222222</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>5.55555555E8</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>